<commit_message>
- fix reference typo in an older dataset
</commit_message>
<xml_diff>
--- a/DatasetForML_Wang2023_Hardness_CompilationAndOriginal.xlsx
+++ b/DatasetForML_Wang2023_Hardness_CompilationAndOriginal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute-Detor2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC664B7-8A74-DF4A-B84E-445FA3C80EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EA7AEA-1DC3-294E-B242-28E497A06987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1425,9 +1425,6 @@
   </si>
   <si>
     <t>10.1103/PhysRevLett.87.156401</t>
-  </si>
-  <si>
-    <t>10.1103/PhysRevLett.65.353</t>
   </si>
   <si>
     <t>10.1038/s41524-019-0151-x</t>
@@ -1583,6 +1580,9 @@
   </si>
   <si>
     <t>All data from Supplementary of 10.1016/j.ijrmhm.2023.106246</t>
+  </si>
+  <si>
+    <t>10.1007/s11837-013-0776-z</t>
   </si>
 </sst>
 </file>
@@ -2265,6 +2265,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2316,34 +2344,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2627,8 +2627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R165" sqref="R165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2664,21 +2664,21 @@
       <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="38" t="s">
-        <v>475</v>
-      </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="49"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2688,17 +2688,17 @@
       <c r="B3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="51"/>
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2716,43 +2716,43 @@
       <c r="B5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="55" t="s">
-        <v>469</v>
-      </c>
-      <c r="N5" s="55" t="s">
+      <c r="M5" s="45" t="s">
+        <v>468</v>
+      </c>
+      <c r="N5" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="39" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2763,19 +2763,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="57"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="40"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2820,12 +2820,12 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="41"/>
       <c r="P7" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q7" s="23" t="s">
         <v>467</v>
-      </c>
-      <c r="Q7" s="23" t="s">
-        <v>468</v>
       </c>
       <c r="R7" s="23" t="s">
         <v>40</v>
@@ -2833,35 +2833,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="53"/>
+      <c r="N8" s="63"/>
       <c r="O8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="44"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2952,12 +2952,12 @@
         <v>42</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N10" t="s">
         <v>440</v>
       </c>
-      <c r="P10" s="64">
+      <c r="P10" s="38">
         <v>220</v>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
         <v>42</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N11" t="s">
         <v>440</v>
       </c>
-      <c r="P11" s="64">
+      <c r="P11" s="38">
         <v>412</v>
       </c>
     </row>
@@ -3028,12 +3028,12 @@
         <v>42</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N12" t="s">
         <v>440</v>
       </c>
-      <c r="P12" s="64">
+      <c r="P12" s="38">
         <v>166</v>
       </c>
     </row>
@@ -3066,13 +3066,13 @@
         <v>42</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N13" t="s">
         <v>441</v>
       </c>
       <c r="O13" s="20"/>
-      <c r="P13" s="64">
+      <c r="P13" s="38">
         <v>353</v>
       </c>
     </row>
@@ -3105,12 +3105,12 @@
         <v>42</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N14" t="s">
         <v>441</v>
       </c>
-      <c r="P14" s="64">
+      <c r="P14" s="38">
         <v>359.6</v>
       </c>
     </row>
@@ -3143,12 +3143,12 @@
         <v>42</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N15" t="s">
         <v>441</v>
       </c>
-      <c r="P15" s="64">
+      <c r="P15" s="38">
         <v>371.6</v>
       </c>
     </row>
@@ -3181,12 +3181,12 @@
         <v>42</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N16" t="s">
         <v>441</v>
       </c>
-      <c r="P16" s="64">
+      <c r="P16" s="38">
         <v>386</v>
       </c>
     </row>
@@ -3219,12 +3219,12 @@
         <v>42</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N17" t="s">
         <v>442</v>
       </c>
-      <c r="P17" s="64">
+      <c r="P17" s="38">
         <v>118</v>
       </c>
     </row>
@@ -3257,12 +3257,12 @@
         <v>42</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N18" t="s">
         <v>442</v>
       </c>
-      <c r="P18" s="64">
+      <c r="P18" s="38">
         <v>127</v>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
         <v>42</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N19" t="s">
         <v>442</v>
       </c>
-      <c r="P19" s="64">
+      <c r="P19" s="38">
         <v>382</v>
       </c>
     </row>
@@ -3333,12 +3333,12 @@
         <v>42</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N20" t="s">
         <v>442</v>
       </c>
-      <c r="P20" s="64">
+      <c r="P20" s="38">
         <v>527</v>
       </c>
     </row>
@@ -3371,12 +3371,12 @@
         <v>42</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N21" t="s">
         <v>442</v>
       </c>
-      <c r="P21" s="64">
+      <c r="P21" s="38">
         <v>482</v>
       </c>
     </row>
@@ -3409,12 +3409,12 @@
         <v>42</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N22" t="s">
         <v>443</v>
       </c>
-      <c r="P22" s="64">
+      <c r="P22" s="38">
         <v>509</v>
       </c>
     </row>
@@ -3447,12 +3447,12 @@
         <v>42</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N23" t="s">
         <v>443</v>
       </c>
-      <c r="P23" s="64">
+      <c r="P23" s="38">
         <v>131</v>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
         <v>42</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N24" t="s">
         <v>443</v>
       </c>
-      <c r="P24" s="64">
+      <c r="P24" s="38">
         <v>388</v>
       </c>
     </row>
@@ -3523,12 +3523,12 @@
         <v>42</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N25" t="s">
         <v>443</v>
       </c>
-      <c r="P25" s="64">
+      <c r="P25" s="38">
         <v>538</v>
       </c>
     </row>
@@ -3561,12 +3561,12 @@
         <v>42</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N26" t="s">
         <v>443</v>
       </c>
-      <c r="P26" s="64">
+      <c r="P26" s="38">
         <v>487</v>
       </c>
     </row>
@@ -3599,12 +3599,12 @@
         <v>42</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N27" t="s">
         <v>444</v>
       </c>
-      <c r="P27" s="64">
+      <c r="P27" s="38">
         <v>135</v>
       </c>
     </row>
@@ -3637,12 +3637,12 @@
         <v>42</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N28" t="s">
         <v>444</v>
       </c>
-      <c r="P28" s="64">
+      <c r="P28" s="38">
         <v>205</v>
       </c>
     </row>
@@ -3675,12 +3675,12 @@
         <v>42</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N29" t="s">
         <v>444</v>
       </c>
-      <c r="P29" s="64">
+      <c r="P29" s="38">
         <v>380</v>
       </c>
     </row>
@@ -3713,12 +3713,12 @@
         <v>42</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N30" t="s">
         <v>445</v>
       </c>
-      <c r="P30" s="64">
+      <c r="P30" s="38">
         <v>150</v>
       </c>
     </row>
@@ -3751,12 +3751,12 @@
         <v>42</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N31" t="s">
         <v>445</v>
       </c>
-      <c r="P31" s="64">
+      <c r="P31" s="38">
         <v>300</v>
       </c>
     </row>
@@ -3789,12 +3789,12 @@
         <v>42</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N32" t="s">
         <v>445</v>
       </c>
-      <c r="P32" s="64">
+      <c r="P32" s="38">
         <v>420</v>
       </c>
     </row>
@@ -3827,12 +3827,12 @@
         <v>42</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N33" t="s">
         <v>446</v>
       </c>
-      <c r="P33" s="64">
+      <c r="P33" s="38">
         <v>238</v>
       </c>
     </row>
@@ -3865,12 +3865,12 @@
         <v>42</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N34" t="s">
         <v>446</v>
       </c>
-      <c r="P34" s="64">
+      <c r="P34" s="38">
         <v>278</v>
       </c>
     </row>
@@ -3903,12 +3903,12 @@
         <v>42</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N35" t="s">
         <v>446</v>
       </c>
-      <c r="P35" s="64">
+      <c r="P35" s="38">
         <v>392</v>
       </c>
     </row>
@@ -3941,12 +3941,12 @@
         <v>42</v>
       </c>
       <c r="M36" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N36" t="s">
         <v>446</v>
       </c>
-      <c r="P36" s="64">
+      <c r="P36" s="38">
         <v>521</v>
       </c>
     </row>
@@ -3979,12 +3979,12 @@
         <v>42</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N37" t="s">
         <v>446</v>
       </c>
-      <c r="P37" s="64">
+      <c r="P37" s="38">
         <v>546</v>
       </c>
     </row>
@@ -4017,12 +4017,12 @@
         <v>42</v>
       </c>
       <c r="M38" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N38" t="s">
         <v>446</v>
       </c>
-      <c r="P38" s="64">
+      <c r="P38" s="38">
         <v>550</v>
       </c>
     </row>
@@ -4055,12 +4055,12 @@
         <v>42</v>
       </c>
       <c r="M39" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N39" t="s">
         <v>446</v>
       </c>
-      <c r="P39" s="64">
+      <c r="P39" s="38">
         <v>544</v>
       </c>
     </row>
@@ -4093,12 +4093,12 @@
         <v>42</v>
       </c>
       <c r="M40" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N40" t="s">
         <v>446</v>
       </c>
-      <c r="P40" s="64">
+      <c r="P40" s="38">
         <v>567</v>
       </c>
     </row>
@@ -4131,12 +4131,12 @@
         <v>42</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N41" t="s">
         <v>446</v>
       </c>
-      <c r="P41" s="64">
+      <c r="P41" s="38">
         <v>576</v>
       </c>
     </row>
@@ -4169,12 +4169,12 @@
         <v>42</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N42" t="s">
         <v>446</v>
       </c>
-      <c r="P42" s="64">
+      <c r="P42" s="38">
         <v>593</v>
       </c>
     </row>
@@ -4207,12 +4207,12 @@
         <v>42</v>
       </c>
       <c r="M43" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N43" t="s">
         <v>447</v>
       </c>
-      <c r="P43" s="64">
+      <c r="P43" s="38">
         <v>473</v>
       </c>
     </row>
@@ -4245,12 +4245,12 @@
         <v>42</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N44" t="s">
         <v>447</v>
       </c>
-      <c r="P44" s="64">
+      <c r="P44" s="38">
         <v>367</v>
       </c>
     </row>
@@ -4283,12 +4283,12 @@
         <v>42</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N45" t="s">
         <v>447</v>
       </c>
-      <c r="P45" s="64">
+      <c r="P45" s="38">
         <v>458</v>
       </c>
     </row>
@@ -4321,12 +4321,12 @@
         <v>42</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N46" t="s">
         <v>447</v>
       </c>
-      <c r="P46" s="64">
+      <c r="P46" s="38">
         <v>418</v>
       </c>
     </row>
@@ -4359,12 +4359,12 @@
         <v>42</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N47" t="s">
         <v>447</v>
       </c>
-      <c r="P47" s="64">
+      <c r="P47" s="38">
         <v>423</v>
       </c>
     </row>
@@ -4397,12 +4397,12 @@
         <v>42</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N48" t="s">
         <v>447</v>
       </c>
-      <c r="P48" s="64">
+      <c r="P48" s="38">
         <v>208</v>
       </c>
     </row>
@@ -4435,12 +4435,12 @@
         <v>42</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N49" t="s">
         <v>448</v>
       </c>
-      <c r="P49" s="64">
+      <c r="P49" s="38">
         <v>280</v>
       </c>
     </row>
@@ -4473,12 +4473,12 @@
         <v>42</v>
       </c>
       <c r="M50" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N50" t="s">
         <v>448</v>
       </c>
-      <c r="P50" s="64">
+      <c r="P50" s="38">
         <v>580</v>
       </c>
     </row>
@@ -4511,12 +4511,12 @@
         <v>42</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N51" t="s">
         <v>449</v>
       </c>
-      <c r="P51" s="64">
+      <c r="P51" s="38">
         <v>450</v>
       </c>
     </row>
@@ -4549,12 +4549,12 @@
         <v>42</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N52" t="s">
         <v>449</v>
       </c>
-      <c r="P52" s="64">
+      <c r="P52" s="38">
         <v>304</v>
       </c>
     </row>
@@ -4587,12 +4587,12 @@
         <v>42</v>
       </c>
       <c r="M53" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N53" t="s">
         <v>450</v>
       </c>
-      <c r="P53" s="64">
+      <c r="P53" s="38">
         <v>695</v>
       </c>
     </row>
@@ -4625,12 +4625,12 @@
         <v>42</v>
       </c>
       <c r="M54" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N54" t="s">
         <v>450</v>
       </c>
-      <c r="P54" s="64">
+      <c r="P54" s="38">
         <v>740</v>
       </c>
     </row>
@@ -4663,12 +4663,12 @@
         <v>42</v>
       </c>
       <c r="M55" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N55" t="s">
         <v>451</v>
       </c>
-      <c r="P55" s="64">
+      <c r="P55" s="38">
         <v>479</v>
       </c>
     </row>
@@ -4701,12 +4701,12 @@
         <v>42</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N56" t="s">
         <v>451</v>
       </c>
-      <c r="P56" s="64">
+      <c r="P56" s="38">
         <v>494</v>
       </c>
     </row>
@@ -4739,12 +4739,12 @@
         <v>42</v>
       </c>
       <c r="M57" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N57" t="s">
         <v>451</v>
       </c>
-      <c r="P57" s="64">
+      <c r="P57" s="38">
         <v>486</v>
       </c>
     </row>
@@ -4777,12 +4777,12 @@
         <v>42</v>
       </c>
       <c r="M58" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N58" t="s">
         <v>451</v>
       </c>
-      <c r="P58" s="64">
+      <c r="P58" s="38">
         <v>408</v>
       </c>
     </row>
@@ -4815,12 +4815,12 @@
         <v>42</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N59" t="s">
         <v>451</v>
       </c>
-      <c r="P59" s="64">
+      <c r="P59" s="38">
         <v>370</v>
       </c>
     </row>
@@ -4853,12 +4853,12 @@
         <v>42</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N60" t="s">
         <v>452</v>
       </c>
-      <c r="P60" s="64">
+      <c r="P60" s="38">
         <v>166</v>
       </c>
     </row>
@@ -4891,12 +4891,12 @@
         <v>42</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N61" t="s">
         <v>452</v>
       </c>
-      <c r="P61" s="64">
+      <c r="P61" s="38">
         <v>536</v>
       </c>
     </row>
@@ -4929,12 +4929,12 @@
         <v>42</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N62" t="s">
         <v>452</v>
       </c>
-      <c r="P62" s="64">
+      <c r="P62" s="38">
         <v>531</v>
       </c>
     </row>
@@ -4967,12 +4967,12 @@
         <v>42</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N63" t="s">
         <v>452</v>
       </c>
-      <c r="P63" s="64">
+      <c r="P63" s="38">
         <v>545</v>
       </c>
     </row>
@@ -5005,12 +5005,12 @@
         <v>42</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N64" t="s">
         <v>452</v>
       </c>
-      <c r="P64" s="64">
+      <c r="P64" s="38">
         <v>366</v>
       </c>
     </row>
@@ -5043,12 +5043,12 @@
         <v>42</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N65" t="s">
         <v>452</v>
       </c>
-      <c r="P65" s="64">
+      <c r="P65" s="38">
         <v>249</v>
       </c>
     </row>
@@ -5081,12 +5081,12 @@
         <v>42</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N66" t="s">
         <v>453</v>
       </c>
-      <c r="P66" s="64">
+      <c r="P66" s="38">
         <v>178.6</v>
       </c>
     </row>
@@ -5119,12 +5119,12 @@
         <v>42</v>
       </c>
       <c r="M67" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N67" t="s">
         <v>453</v>
       </c>
-      <c r="P67" s="64">
+      <c r="P67" s="38">
         <v>169.7</v>
       </c>
     </row>
@@ -5157,12 +5157,12 @@
         <v>42</v>
       </c>
       <c r="M68" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N68" t="s">
         <v>453</v>
       </c>
-      <c r="P68" s="64">
+      <c r="P68" s="38">
         <v>182</v>
       </c>
     </row>
@@ -5195,12 +5195,12 @@
         <v>42</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N69" t="s">
         <v>453</v>
       </c>
-      <c r="P69" s="64">
+      <c r="P69" s="38">
         <v>182.5</v>
       </c>
     </row>
@@ -5233,12 +5233,12 @@
         <v>42</v>
       </c>
       <c r="M70" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N70" t="s">
         <v>453</v>
       </c>
-      <c r="P70" s="64">
+      <c r="P70" s="38">
         <v>218.9</v>
       </c>
     </row>
@@ -5271,12 +5271,12 @@
         <v>42</v>
       </c>
       <c r="M71" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N71" t="s">
         <v>453</v>
       </c>
-      <c r="P71" s="64">
+      <c r="P71" s="38">
         <v>277.8</v>
       </c>
     </row>
@@ -5309,12 +5309,12 @@
         <v>42</v>
       </c>
       <c r="M72" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N72" t="s">
         <v>453</v>
       </c>
-      <c r="P72" s="64">
+      <c r="P72" s="38">
         <v>402.6</v>
       </c>
     </row>
@@ -5346,12 +5346,12 @@
         <v>42</v>
       </c>
       <c r="M73" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N73" t="s">
         <v>453</v>
       </c>
-      <c r="P73" s="64">
+      <c r="P73" s="38">
         <v>484.1</v>
       </c>
     </row>
@@ -5383,12 +5383,12 @@
         <v>42</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N74" t="s">
         <v>453</v>
       </c>
-      <c r="P74" s="64">
+      <c r="P74" s="38">
         <v>528.29999999999995</v>
       </c>
     </row>
@@ -5420,12 +5420,12 @@
         <v>42</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N75" t="s">
         <v>453</v>
       </c>
-      <c r="P75" s="64">
+      <c r="P75" s="38">
         <v>538.1</v>
       </c>
     </row>
@@ -5457,12 +5457,12 @@
         <v>42</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N76" t="s">
         <v>453</v>
       </c>
-      <c r="P76" s="64">
+      <c r="P76" s="38">
         <v>530.29999999999995</v>
       </c>
     </row>
@@ -5494,12 +5494,12 @@
         <v>42</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N77" t="s">
         <v>453</v>
       </c>
-      <c r="P77" s="64">
+      <c r="P77" s="38">
         <v>534.20000000000005</v>
       </c>
     </row>
@@ -5531,12 +5531,12 @@
         <v>42</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N78" t="s">
         <v>453</v>
       </c>
-      <c r="P78" s="64">
+      <c r="P78" s="38">
         <v>537.1</v>
       </c>
     </row>
@@ -5568,12 +5568,12 @@
         <v>42</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N79" t="s">
         <v>454</v>
       </c>
-      <c r="P79" s="64">
+      <c r="P79" s="38">
         <v>168</v>
       </c>
     </row>
@@ -5605,12 +5605,12 @@
         <v>42</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N80" t="s">
         <v>455</v>
       </c>
-      <c r="P80" s="64">
+      <c r="P80" s="38">
         <v>273</v>
       </c>
     </row>
@@ -5642,12 +5642,12 @@
         <v>42</v>
       </c>
       <c r="M81" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N81" t="s">
         <v>455</v>
       </c>
-      <c r="P81" s="64">
+      <c r="P81" s="38">
         <v>475</v>
       </c>
     </row>
@@ -5679,12 +5679,12 @@
         <v>42</v>
       </c>
       <c r="M82" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N82" t="s">
         <v>455</v>
       </c>
-      <c r="P82" s="64">
+      <c r="P82" s="38">
         <v>558</v>
       </c>
     </row>
@@ -5716,12 +5716,12 @@
         <v>42</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N83" t="s">
         <v>455</v>
       </c>
-      <c r="P83" s="64">
+      <c r="P83" s="38">
         <v>510</v>
       </c>
     </row>
@@ -5753,12 +5753,12 @@
         <v>42</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N84" t="s">
         <v>455</v>
       </c>
-      <c r="P84" s="64">
+      <c r="P84" s="38">
         <v>603</v>
       </c>
     </row>
@@ -5790,12 +5790,12 @@
         <v>42</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N85" t="s">
         <v>455</v>
       </c>
-      <c r="P85" s="64">
+      <c r="P85" s="38">
         <v>625</v>
       </c>
     </row>
@@ -5827,12 +5827,12 @@
         <v>42</v>
       </c>
       <c r="M86" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N86" t="s">
         <v>455</v>
       </c>
-      <c r="P86" s="64">
+      <c r="P86" s="38">
         <v>655</v>
       </c>
     </row>
@@ -5864,12 +5864,12 @@
         <v>42</v>
       </c>
       <c r="M87" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N87" t="s">
         <v>455</v>
       </c>
-      <c r="P87" s="64">
+      <c r="P87" s="38">
         <v>735</v>
       </c>
     </row>
@@ -5901,12 +5901,12 @@
         <v>42</v>
       </c>
       <c r="M88" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N88" t="s">
         <v>456</v>
       </c>
-      <c r="P88" s="64">
+      <c r="P88" s="38">
         <v>152</v>
       </c>
     </row>
@@ -5938,12 +5938,12 @@
         <v>42</v>
       </c>
       <c r="M89" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N89" t="s">
         <v>457</v>
       </c>
-      <c r="P89" s="64">
+      <c r="P89" s="38">
         <v>286</v>
       </c>
     </row>
@@ -5975,12 +5975,12 @@
         <v>42</v>
       </c>
       <c r="M90" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N90" t="s">
         <v>458</v>
       </c>
-      <c r="P90" s="64">
+      <c r="P90" s="38">
         <v>358</v>
       </c>
     </row>
@@ -6012,12 +6012,12 @@
         <v>42</v>
       </c>
       <c r="M91" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N91" t="s">
         <v>458</v>
       </c>
-      <c r="P91" s="64">
+      <c r="P91" s="38">
         <v>586</v>
       </c>
     </row>
@@ -6049,12 +6049,12 @@
         <v>42</v>
       </c>
       <c r="M92" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N92" t="s">
         <v>458</v>
       </c>
-      <c r="P92" s="64">
+      <c r="P92" s="38">
         <v>601</v>
       </c>
     </row>
@@ -6086,12 +6086,12 @@
         <v>42</v>
       </c>
       <c r="M93" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N93" t="s">
         <v>458</v>
       </c>
-      <c r="P93" s="64">
+      <c r="P93" s="38">
         <v>295</v>
       </c>
     </row>
@@ -6123,12 +6123,12 @@
         <v>42</v>
       </c>
       <c r="M94" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N94" t="s">
         <v>458</v>
       </c>
-      <c r="P94" s="64">
+      <c r="P94" s="38">
         <v>584</v>
       </c>
     </row>
@@ -6160,12 +6160,12 @@
         <v>42</v>
       </c>
       <c r="M95" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N95" t="s">
         <v>458</v>
       </c>
-      <c r="P95" s="64">
+      <c r="P95" s="38">
         <v>310</v>
       </c>
     </row>
@@ -6197,12 +6197,12 @@
         <v>42</v>
       </c>
       <c r="M96" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N96" t="s">
         <v>458</v>
       </c>
-      <c r="P96" s="64">
+      <c r="P96" s="38">
         <v>451</v>
       </c>
     </row>
@@ -6234,12 +6234,12 @@
         <v>42</v>
       </c>
       <c r="M97" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N97" t="s">
         <v>458</v>
       </c>
-      <c r="P97" s="64">
+      <c r="P97" s="38">
         <v>546</v>
       </c>
     </row>
@@ -6271,12 +6271,12 @@
         <v>42</v>
       </c>
       <c r="M98" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N98" t="s">
         <v>458</v>
       </c>
-      <c r="P98" s="64">
+      <c r="P98" s="38">
         <v>607</v>
       </c>
     </row>
@@ -6308,12 +6308,12 @@
         <v>42</v>
       </c>
       <c r="M99" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N99" t="s">
         <v>458</v>
       </c>
-      <c r="P99" s="64">
+      <c r="P99" s="38">
         <v>537</v>
       </c>
     </row>
@@ -6345,12 +6345,12 @@
         <v>42</v>
       </c>
       <c r="M100" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N100" t="s">
         <v>458</v>
       </c>
-      <c r="P100" s="64">
+      <c r="P100" s="38">
         <v>514</v>
       </c>
     </row>
@@ -6382,12 +6382,12 @@
         <v>42</v>
       </c>
       <c r="M101" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N101" t="s">
         <v>458</v>
       </c>
-      <c r="P101" s="64">
+      <c r="P101" s="38">
         <v>604</v>
       </c>
     </row>
@@ -6419,12 +6419,12 @@
         <v>42</v>
       </c>
       <c r="M102" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N102" t="s">
         <v>458</v>
       </c>
-      <c r="P102" s="64">
+      <c r="P102" s="38">
         <v>639</v>
       </c>
     </row>
@@ -6456,12 +6456,12 @@
         <v>42</v>
       </c>
       <c r="M103" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N103" t="s">
         <v>458</v>
       </c>
-      <c r="P103" s="64">
+      <c r="P103" s="38">
         <v>534</v>
       </c>
     </row>
@@ -6493,12 +6493,12 @@
         <v>42</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N104" t="s">
         <v>458</v>
       </c>
-      <c r="P104" s="64">
+      <c r="P104" s="38">
         <v>609</v>
       </c>
     </row>
@@ -6530,12 +6530,12 @@
         <v>42</v>
       </c>
       <c r="M105" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N105" t="s">
         <v>458</v>
       </c>
-      <c r="P105" s="64">
+      <c r="P105" s="38">
         <v>551</v>
       </c>
     </row>
@@ -6567,12 +6567,12 @@
         <v>42</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N106" t="s">
         <v>458</v>
       </c>
-      <c r="P106" s="64">
+      <c r="P106" s="38">
         <v>586</v>
       </c>
     </row>
@@ -6604,12 +6604,12 @@
         <v>42</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N107" t="s">
         <v>459</v>
       </c>
-      <c r="P107" s="64">
+      <c r="P107" s="38">
         <v>225</v>
       </c>
     </row>
@@ -6641,12 +6641,12 @@
         <v>42</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N108" t="s">
         <v>459</v>
       </c>
-      <c r="P108" s="64">
+      <c r="P108" s="38">
         <v>146</v>
       </c>
     </row>
@@ -6678,12 +6678,12 @@
         <v>42</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N109" t="s">
         <v>459</v>
       </c>
-      <c r="P109" s="64">
+      <c r="P109" s="38">
         <v>150</v>
       </c>
     </row>
@@ -6715,12 +6715,12 @@
         <v>42</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N110" t="s">
         <v>459</v>
       </c>
-      <c r="P110" s="64">
+      <c r="P110" s="38">
         <v>158</v>
       </c>
     </row>
@@ -6752,12 +6752,12 @@
         <v>42</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N111" t="s">
         <v>459</v>
       </c>
-      <c r="P111" s="64">
+      <c r="P111" s="38">
         <v>175</v>
       </c>
     </row>
@@ -6789,12 +6789,12 @@
         <v>42</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N112" t="s">
         <v>459</v>
       </c>
-      <c r="P112" s="64">
+      <c r="P112" s="38">
         <v>154</v>
       </c>
     </row>
@@ -6826,12 +6826,12 @@
         <v>42</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N113" t="s">
         <v>459</v>
       </c>
-      <c r="P113" s="64">
+      <c r="P113" s="38">
         <v>153</v>
       </c>
     </row>
@@ -6863,12 +6863,12 @@
         <v>42</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N114" t="s">
         <v>459</v>
       </c>
-      <c r="P114" s="64">
+      <c r="P114" s="38">
         <v>158</v>
       </c>
     </row>
@@ -6900,12 +6900,12 @@
         <v>42</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N115" t="s">
         <v>459</v>
       </c>
-      <c r="P115" s="64">
+      <c r="P115" s="38">
         <v>161</v>
       </c>
     </row>
@@ -6937,12 +6937,12 @@
         <v>42</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N116" t="s">
         <v>459</v>
       </c>
-      <c r="P116" s="64">
+      <c r="P116" s="38">
         <v>172</v>
       </c>
     </row>
@@ -6974,12 +6974,12 @@
         <v>42</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N117" t="s">
         <v>459</v>
       </c>
-      <c r="P117" s="64">
+      <c r="P117" s="38">
         <v>183</v>
       </c>
     </row>
@@ -7011,12 +7011,12 @@
         <v>42</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N118" t="s">
         <v>459</v>
       </c>
-      <c r="P118" s="64">
+      <c r="P118" s="38">
         <v>182</v>
       </c>
     </row>
@@ -7048,12 +7048,12 @@
         <v>42</v>
       </c>
       <c r="M119" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N119" t="s">
         <v>459</v>
       </c>
-      <c r="P119" s="64">
+      <c r="P119" s="38">
         <v>172</v>
       </c>
     </row>
@@ -7085,12 +7085,12 @@
         <v>42</v>
       </c>
       <c r="M120" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N120" t="s">
         <v>459</v>
       </c>
-      <c r="P120" s="64">
+      <c r="P120" s="38">
         <v>157</v>
       </c>
     </row>
@@ -7122,12 +7122,12 @@
         <v>42</v>
       </c>
       <c r="M121" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N121" t="s">
         <v>459</v>
       </c>
-      <c r="P121" s="64">
+      <c r="P121" s="38">
         <v>170</v>
       </c>
     </row>
@@ -7159,12 +7159,12 @@
         <v>42</v>
       </c>
       <c r="M122" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N122" t="s">
         <v>459</v>
       </c>
-      <c r="P122" s="64">
+      <c r="P122" s="38">
         <v>167</v>
       </c>
     </row>
@@ -7196,12 +7196,12 @@
         <v>42</v>
       </c>
       <c r="M123" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N123" t="s">
         <v>459</v>
       </c>
-      <c r="P123" s="64">
+      <c r="P123" s="38">
         <v>158</v>
       </c>
     </row>
@@ -7233,12 +7233,12 @@
         <v>42</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N124" t="s">
         <v>459</v>
       </c>
-      <c r="P124" s="64">
+      <c r="P124" s="38">
         <v>140</v>
       </c>
     </row>
@@ -7270,12 +7270,12 @@
         <v>42</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N125" t="s">
         <v>459</v>
       </c>
-      <c r="P125" s="64">
+      <c r="P125" s="38">
         <v>125</v>
       </c>
     </row>
@@ -7307,12 +7307,12 @@
         <v>42</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N126" t="s">
         <v>459</v>
       </c>
-      <c r="P126" s="64">
+      <c r="P126" s="38">
         <v>242</v>
       </c>
     </row>
@@ -7344,12 +7344,12 @@
         <v>42</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N127" t="s">
         <v>459</v>
       </c>
-      <c r="P127" s="64">
+      <c r="P127" s="38">
         <v>265</v>
       </c>
     </row>
@@ -7381,12 +7381,12 @@
         <v>42</v>
       </c>
       <c r="M128" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N128" t="s">
         <v>459</v>
       </c>
-      <c r="P128" s="64">
+      <c r="P128" s="38">
         <v>335</v>
       </c>
     </row>
@@ -7418,12 +7418,12 @@
         <v>42</v>
       </c>
       <c r="M129" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N129" t="s">
         <v>459</v>
       </c>
-      <c r="P129" s="64">
+      <c r="P129" s="38">
         <v>170</v>
       </c>
     </row>
@@ -7455,12 +7455,12 @@
         <v>42</v>
       </c>
       <c r="M130" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N130" t="s">
         <v>459</v>
       </c>
-      <c r="P130" s="64">
+      <c r="P130" s="38">
         <v>503</v>
       </c>
     </row>
@@ -7492,12 +7492,12 @@
         <v>42</v>
       </c>
       <c r="M131" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N131" t="s">
         <v>459</v>
       </c>
-      <c r="P131" s="64">
+      <c r="P131" s="38">
         <v>555</v>
       </c>
     </row>
@@ -7529,12 +7529,12 @@
         <v>42</v>
       </c>
       <c r="M132" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N132" t="s">
         <v>459</v>
       </c>
-      <c r="P132" s="64">
+      <c r="P132" s="38">
         <v>548</v>
       </c>
     </row>
@@ -7566,12 +7566,12 @@
         <v>42</v>
       </c>
       <c r="M133" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N133" t="s">
         <v>459</v>
       </c>
-      <c r="P133" s="64">
+      <c r="P133" s="38">
         <v>615</v>
       </c>
     </row>
@@ -7603,12 +7603,12 @@
         <v>42</v>
       </c>
       <c r="M134" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N134" t="s">
         <v>459</v>
       </c>
-      <c r="P134" s="64">
+      <c r="P134" s="38">
         <v>720</v>
       </c>
     </row>
@@ -7640,12 +7640,12 @@
         <v>42</v>
       </c>
       <c r="M135" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N135" t="s">
         <v>459</v>
       </c>
-      <c r="P135" s="64">
+      <c r="P135" s="38">
         <v>550</v>
       </c>
     </row>
@@ -7677,12 +7677,12 @@
         <v>42</v>
       </c>
       <c r="M136" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N136" t="s">
         <v>459</v>
       </c>
-      <c r="P136" s="64">
+      <c r="P136" s="38">
         <v>539</v>
       </c>
     </row>
@@ -7714,12 +7714,12 @@
         <v>42</v>
       </c>
       <c r="M137" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N137" t="s">
         <v>459</v>
       </c>
-      <c r="P137" s="64">
+      <c r="P137" s="38">
         <v>438</v>
       </c>
     </row>
@@ -7751,12 +7751,12 @@
         <v>42</v>
       </c>
       <c r="M138" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N138" t="s">
         <v>459</v>
       </c>
-      <c r="P138" s="64">
+      <c r="P138" s="38">
         <v>476</v>
       </c>
     </row>
@@ -7788,12 +7788,12 @@
         <v>42</v>
       </c>
       <c r="M139" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N139" t="s">
         <v>459</v>
       </c>
-      <c r="P139" s="64">
+      <c r="P139" s="38">
         <v>587</v>
       </c>
     </row>
@@ -7825,12 +7825,12 @@
         <v>42</v>
       </c>
       <c r="M140" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N140" t="s">
         <v>459</v>
       </c>
-      <c r="P140" s="64">
+      <c r="P140" s="38">
         <v>558</v>
       </c>
     </row>
@@ -7862,12 +7862,12 @@
         <v>42</v>
       </c>
       <c r="M141" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N141" t="s">
         <v>459</v>
       </c>
-      <c r="P141" s="64">
+      <c r="P141" s="38">
         <v>510</v>
       </c>
     </row>
@@ -7899,12 +7899,12 @@
         <v>42</v>
       </c>
       <c r="M142" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N142" t="s">
         <v>459</v>
       </c>
-      <c r="P142" s="64">
+      <c r="P142" s="38">
         <v>775</v>
       </c>
     </row>
@@ -7936,12 +7936,12 @@
         <v>42</v>
       </c>
       <c r="M143" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N143" t="s">
         <v>459</v>
       </c>
-      <c r="P143" s="64">
+      <c r="P143" s="38">
         <v>140</v>
       </c>
     </row>
@@ -7973,12 +7973,12 @@
         <v>42</v>
       </c>
       <c r="M144" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N144" t="s">
         <v>459</v>
       </c>
-      <c r="P144" s="64">
+      <c r="P144" s="38">
         <v>410</v>
       </c>
     </row>
@@ -8010,12 +8010,12 @@
         <v>42</v>
       </c>
       <c r="M145" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N145" t="s">
         <v>459</v>
       </c>
-      <c r="P145" s="64">
+      <c r="P145" s="38">
         <v>510</v>
       </c>
     </row>
@@ -8047,12 +8047,12 @@
         <v>42</v>
       </c>
       <c r="M146" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N146" t="s">
         <v>460</v>
       </c>
-      <c r="P146" s="64">
+      <c r="P146" s="38">
         <v>145</v>
       </c>
     </row>
@@ -8084,12 +8084,12 @@
         <v>42</v>
       </c>
       <c r="M147" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N147" t="s">
         <v>461</v>
       </c>
-      <c r="P147" s="64">
+      <c r="P147" s="38">
         <v>359</v>
       </c>
     </row>
@@ -8121,12 +8121,12 @@
         <v>42</v>
       </c>
       <c r="M148" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N148" t="s">
         <v>462</v>
       </c>
-      <c r="P148" s="64">
+      <c r="P148" s="38">
         <v>396</v>
       </c>
     </row>
@@ -8158,12 +8158,12 @@
         <v>42</v>
       </c>
       <c r="M149" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N149" t="s">
-        <v>463</v>
-      </c>
-      <c r="P149" s="64">
+        <v>475</v>
+      </c>
+      <c r="P149" s="38">
         <v>271</v>
       </c>
     </row>
@@ -8195,12 +8195,12 @@
         <v>42</v>
       </c>
       <c r="M150" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N150" t="s">
-        <v>463</v>
-      </c>
-      <c r="P150" s="64">
+        <v>475</v>
+      </c>
+      <c r="P150" s="38">
         <v>406</v>
       </c>
     </row>
@@ -8232,12 +8232,12 @@
         <v>42</v>
       </c>
       <c r="M151" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N151" t="s">
-        <v>463</v>
-      </c>
-      <c r="P151" s="64">
+        <v>475</v>
+      </c>
+      <c r="P151" s="38">
         <v>481</v>
       </c>
     </row>
@@ -8269,12 +8269,12 @@
         <v>42</v>
       </c>
       <c r="M152" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N152" t="s">
-        <v>463</v>
-      </c>
-      <c r="P152" s="64">
+        <v>475</v>
+      </c>
+      <c r="P152" s="38">
         <v>661</v>
       </c>
     </row>
@@ -8306,12 +8306,12 @@
         <v>42</v>
       </c>
       <c r="M153" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N153" t="s">
-        <v>463</v>
-      </c>
-      <c r="P153" s="64">
+        <v>475</v>
+      </c>
+      <c r="P153" s="38">
         <v>240</v>
       </c>
     </row>
@@ -8343,12 +8343,12 @@
         <v>42</v>
       </c>
       <c r="M154" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N154" t="s">
-        <v>463</v>
-      </c>
-      <c r="P154" s="64">
+        <v>475</v>
+      </c>
+      <c r="P154" s="38">
         <v>328</v>
       </c>
     </row>
@@ -8380,12 +8380,12 @@
         <v>42</v>
       </c>
       <c r="M155" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N155" t="s">
-        <v>463</v>
-      </c>
-      <c r="P155" s="64">
+        <v>475</v>
+      </c>
+      <c r="P155" s="38">
         <v>379</v>
       </c>
     </row>
@@ -8417,12 +8417,12 @@
         <v>42</v>
       </c>
       <c r="M156" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N156" t="s">
-        <v>463</v>
-      </c>
-      <c r="P156" s="64">
+        <v>475</v>
+      </c>
+      <c r="P156" s="38">
         <v>481</v>
       </c>
     </row>
@@ -8454,12 +8454,12 @@
         <v>42</v>
       </c>
       <c r="M157" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N157" t="s">
-        <v>463</v>
-      </c>
-      <c r="P157" s="64">
+        <v>475</v>
+      </c>
+      <c r="P157" s="38">
         <v>484</v>
       </c>
     </row>
@@ -8491,12 +8491,12 @@
         <v>42</v>
       </c>
       <c r="M158" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N158" t="s">
-        <v>463</v>
-      </c>
-      <c r="P158" s="64">
+        <v>475</v>
+      </c>
+      <c r="P158" s="38">
         <v>740</v>
       </c>
     </row>
@@ -8528,12 +8528,12 @@
         <v>42</v>
       </c>
       <c r="M159" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N159" t="s">
-        <v>463</v>
-      </c>
-      <c r="P159" s="64">
+        <v>475</v>
+      </c>
+      <c r="P159" s="38">
         <v>169</v>
       </c>
     </row>
@@ -8565,12 +8565,12 @@
         <v>42</v>
       </c>
       <c r="M160" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N160" t="s">
-        <v>463</v>
-      </c>
-      <c r="P160" s="64">
+        <v>475</v>
+      </c>
+      <c r="P160" s="38">
         <v>200</v>
       </c>
     </row>
@@ -8602,12 +8602,12 @@
         <v>42</v>
       </c>
       <c r="M161" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N161" t="s">
-        <v>463</v>
-      </c>
-      <c r="P161" s="64">
+        <v>475</v>
+      </c>
+      <c r="P161" s="38">
         <v>240</v>
       </c>
     </row>
@@ -8639,12 +8639,12 @@
         <v>42</v>
       </c>
       <c r="M162" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N162" t="s">
-        <v>463</v>
-      </c>
-      <c r="P162" s="64">
+        <v>475</v>
+      </c>
+      <c r="P162" s="38">
         <v>291</v>
       </c>
     </row>
@@ -8676,12 +8676,12 @@
         <v>42</v>
       </c>
       <c r="M163" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N163" t="s">
-        <v>463</v>
-      </c>
-      <c r="P163" s="64">
+        <v>475</v>
+      </c>
+      <c r="P163" s="38">
         <v>322</v>
       </c>
     </row>
@@ -8713,12 +8713,12 @@
         <v>42</v>
       </c>
       <c r="M164" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N164" t="s">
-        <v>463</v>
-      </c>
-      <c r="P164" s="64">
+        <v>475</v>
+      </c>
+      <c r="P164" s="38">
         <v>338</v>
       </c>
     </row>
@@ -8750,12 +8750,12 @@
         <v>42</v>
       </c>
       <c r="M165" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N165" t="s">
-        <v>463</v>
-      </c>
-      <c r="P165" s="64">
+        <v>475</v>
+      </c>
+      <c r="P165" s="38">
         <v>389</v>
       </c>
     </row>
@@ -8787,12 +8787,12 @@
         <v>42</v>
       </c>
       <c r="M166" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N166" t="s">
-        <v>463</v>
-      </c>
-      <c r="P166" s="64">
+        <v>475</v>
+      </c>
+      <c r="P166" s="38">
         <v>522</v>
       </c>
     </row>
@@ -8824,12 +8824,12 @@
         <v>42</v>
       </c>
       <c r="M167" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N167" t="s">
-        <v>463</v>
-      </c>
-      <c r="P167" s="64">
+        <v>475</v>
+      </c>
+      <c r="P167" s="38">
         <v>572</v>
       </c>
     </row>
@@ -8861,12 +8861,12 @@
         <v>42</v>
       </c>
       <c r="M168" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N168" t="s">
-        <v>463</v>
-      </c>
-      <c r="P168" s="64">
+        <v>475</v>
+      </c>
+      <c r="P168" s="38">
         <v>600</v>
       </c>
     </row>
@@ -8898,12 +8898,12 @@
         <v>42</v>
       </c>
       <c r="M169" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N169" t="s">
-        <v>464</v>
-      </c>
-      <c r="P169" s="64">
+        <v>463</v>
+      </c>
+      <c r="P169" s="38">
         <v>154</v>
       </c>
     </row>
@@ -8935,12 +8935,12 @@
         <v>42</v>
       </c>
       <c r="M170" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N170" t="s">
-        <v>465</v>
-      </c>
-      <c r="P170" s="64">
+        <v>464</v>
+      </c>
+      <c r="P170" s="38">
         <v>419</v>
       </c>
     </row>
@@ -8972,12 +8972,12 @@
         <v>42</v>
       </c>
       <c r="M171" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N171" t="s">
-        <v>466</v>
-      </c>
-      <c r="P171" s="64">
+        <v>465</v>
+      </c>
+      <c r="P171" s="38">
         <v>764</v>
       </c>
     </row>
@@ -9009,12 +9009,12 @@
         <v>42</v>
       </c>
       <c r="M172" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N172" t="s">
-        <v>466</v>
-      </c>
-      <c r="P172" s="64">
+        <v>465</v>
+      </c>
+      <c r="P172" s="38">
         <v>591</v>
       </c>
     </row>
@@ -9046,12 +9046,12 @@
         <v>42</v>
       </c>
       <c r="M173" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N173" t="s">
-        <v>466</v>
-      </c>
-      <c r="P173" s="64">
+        <v>465</v>
+      </c>
+      <c r="P173" s="38">
         <v>701</v>
       </c>
     </row>
@@ -9083,12 +9083,12 @@
         <v>42</v>
       </c>
       <c r="M174" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N174" t="s">
-        <v>466</v>
-      </c>
-      <c r="P174" s="64">
+        <v>465</v>
+      </c>
+      <c r="P174" s="38">
         <v>768</v>
       </c>
     </row>
@@ -9120,12 +9120,12 @@
         <v>42</v>
       </c>
       <c r="M175" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N175" t="s">
-        <v>466</v>
-      </c>
-      <c r="P175" s="64">
+        <v>465</v>
+      </c>
+      <c r="P175" s="38">
         <v>702</v>
       </c>
     </row>
@@ -9157,12 +9157,12 @@
         <v>42</v>
       </c>
       <c r="M176" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N176" t="s">
-        <v>466</v>
-      </c>
-      <c r="P176" s="64">
+        <v>465</v>
+      </c>
+      <c r="P176" s="38">
         <v>694</v>
       </c>
     </row>
@@ -9194,12 +9194,12 @@
         <v>42</v>
       </c>
       <c r="M177" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N177" t="s">
-        <v>466</v>
-      </c>
-      <c r="P177" s="64">
+        <v>465</v>
+      </c>
+      <c r="P177" s="38">
         <v>149</v>
       </c>
     </row>
@@ -9231,12 +9231,12 @@
         <v>42</v>
       </c>
       <c r="M178" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N178" t="s">
-        <v>466</v>
-      </c>
-      <c r="P178" s="64">
+        <v>465</v>
+      </c>
+      <c r="P178" s="38">
         <v>229</v>
       </c>
     </row>
@@ -9268,12 +9268,12 @@
         <v>42</v>
       </c>
       <c r="M179" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N179" t="s">
-        <v>466</v>
-      </c>
-      <c r="P179" s="64">
+        <v>465</v>
+      </c>
+      <c r="P179" s="38">
         <v>459</v>
       </c>
     </row>
@@ -9305,12 +9305,12 @@
         <v>42</v>
       </c>
       <c r="M180" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N180" t="s">
-        <v>466</v>
-      </c>
-      <c r="P180" s="64">
+        <v>465</v>
+      </c>
+      <c r="P180" s="38">
         <v>469</v>
       </c>
     </row>
@@ -9342,12 +9342,12 @@
         <v>42</v>
       </c>
       <c r="M181" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N181" t="s">
-        <v>466</v>
-      </c>
-      <c r="P181" s="64">
+        <v>465</v>
+      </c>
+      <c r="P181" s="38">
         <v>483</v>
       </c>
     </row>
@@ -9379,12 +9379,12 @@
         <v>42</v>
       </c>
       <c r="M182" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N182" t="s">
-        <v>466</v>
-      </c>
-      <c r="P182" s="64">
+        <v>465</v>
+      </c>
+      <c r="P182" s="38">
         <v>472</v>
       </c>
     </row>
@@ -9416,12 +9416,12 @@
         <v>42</v>
       </c>
       <c r="M183" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N183" t="s">
-        <v>466</v>
-      </c>
-      <c r="P183" s="64">
+        <v>465</v>
+      </c>
+      <c r="P183" s="38">
         <v>454</v>
       </c>
     </row>
@@ -9453,12 +9453,12 @@
         <v>42</v>
       </c>
       <c r="M184" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N184" t="s">
-        <v>466</v>
-      </c>
-      <c r="P184" s="64">
+        <v>465</v>
+      </c>
+      <c r="P184" s="38">
         <v>441</v>
       </c>
     </row>
@@ -9490,12 +9490,12 @@
         <v>42</v>
       </c>
       <c r="M185" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N185" t="s">
-        <v>466</v>
-      </c>
-      <c r="P185" s="64">
+        <v>465</v>
+      </c>
+      <c r="P185" s="38">
         <v>495</v>
       </c>
     </row>
@@ -9527,12 +9527,12 @@
         <v>42</v>
       </c>
       <c r="M186" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N186" t="s">
-        <v>466</v>
-      </c>
-      <c r="P186" s="64">
+        <v>465</v>
+      </c>
+      <c r="P186" s="38">
         <v>477</v>
       </c>
     </row>
@@ -9564,12 +9564,12 @@
         <v>42</v>
       </c>
       <c r="M187" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N187" t="s">
-        <v>466</v>
-      </c>
-      <c r="P187" s="64">
+        <v>465</v>
+      </c>
+      <c r="P187" s="38">
         <v>469</v>
       </c>
     </row>
@@ -9582,7 +9582,7 @@
       </c>
       <c r="C188" s="34"/>
       <c r="D188" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F188" s="33" t="s">
         <v>62</v>
@@ -9609,9 +9609,9 @@
         <v>61</v>
       </c>
       <c r="N188" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P188" s="64">
+        <v>470</v>
+      </c>
+      <c r="P188" s="38">
         <v>785.6</v>
       </c>
       <c r="Q188">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="C189" s="34"/>
       <c r="D189" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F189" s="33" t="s">
         <v>62</v>
@@ -9654,9 +9654,9 @@
         <v>61</v>
       </c>
       <c r="N189" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P189" s="64">
+        <v>470</v>
+      </c>
+      <c r="P189" s="38">
         <v>771.1</v>
       </c>
       <c r="Q189">
@@ -9672,7 +9672,7 @@
       </c>
       <c r="C190" s="34"/>
       <c r="D190" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F190" s="33" t="s">
         <v>62</v>
@@ -9699,9 +9699,9 @@
         <v>61</v>
       </c>
       <c r="N190" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P190" s="64">
+        <v>470</v>
+      </c>
+      <c r="P190" s="38">
         <v>783.7</v>
       </c>
       <c r="Q190">
@@ -9717,7 +9717,7 @@
       </c>
       <c r="C191" s="34"/>
       <c r="D191" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F191" s="33" t="s">
         <v>62</v>
@@ -9744,9 +9744,9 @@
         <v>61</v>
       </c>
       <c r="N191" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P191" s="64">
+        <v>470</v>
+      </c>
+      <c r="P191" s="38">
         <v>771.9</v>
       </c>
       <c r="Q191">
@@ -9762,7 +9762,7 @@
       </c>
       <c r="C192" s="34"/>
       <c r="D192" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F192" s="33" t="s">
         <v>62</v>
@@ -9789,9 +9789,9 @@
         <v>61</v>
       </c>
       <c r="N192" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P192" s="64">
+        <v>470</v>
+      </c>
+      <c r="P192" s="38">
         <v>797.1</v>
       </c>
       <c r="Q192">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="C193" s="34"/>
       <c r="D193" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F193" s="33" t="s">
         <v>62</v>
@@ -9834,9 +9834,9 @@
         <v>61</v>
       </c>
       <c r="N193" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P193" s="64">
+        <v>470</v>
+      </c>
+      <c r="P193" s="38">
         <v>792.2</v>
       </c>
       <c r="Q193">
@@ -9852,7 +9852,7 @@
       </c>
       <c r="C194" s="34"/>
       <c r="D194" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F194" s="33" t="s">
         <v>62</v>
@@ -9879,9 +9879,9 @@
         <v>61</v>
       </c>
       <c r="N194" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P194" s="64">
+        <v>470</v>
+      </c>
+      <c r="P194" s="38">
         <v>804.3</v>
       </c>
       <c r="Q194">
@@ -9896,13 +9896,13 @@
         <v>333</v>
       </c>
       <c r="C195" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="D195" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="E195" t="s">
         <v>472</v>
-      </c>
-      <c r="D195" s="34" t="s">
-        <v>474</v>
-      </c>
-      <c r="E195" t="s">
-        <v>473</v>
       </c>
       <c r="F195" s="33" t="s">
         <v>62</v>
@@ -9929,9 +9929,9 @@
         <v>61</v>
       </c>
       <c r="N195" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P195" s="64">
+        <v>470</v>
+      </c>
+      <c r="P195" s="38">
         <v>815.4</v>
       </c>
       <c r="Q195">
@@ -9946,13 +9946,13 @@
         <v>334</v>
       </c>
       <c r="C196" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="D196" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="E196" t="s">
         <v>472</v>
-      </c>
-      <c r="D196" s="34" t="s">
-        <v>474</v>
-      </c>
-      <c r="E196" t="s">
-        <v>473</v>
       </c>
       <c r="F196" s="33" t="s">
         <v>62</v>
@@ -9979,9 +9979,9 @@
         <v>61</v>
       </c>
       <c r="N196" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P196" s="64">
+        <v>470</v>
+      </c>
+      <c r="P196" s="38">
         <v>814.5</v>
       </c>
       <c r="Q196">
@@ -9996,13 +9996,13 @@
         <v>335</v>
       </c>
       <c r="C197" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="D197" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="E197" t="s">
         <v>472</v>
-      </c>
-      <c r="D197" s="34" t="s">
-        <v>474</v>
-      </c>
-      <c r="E197" t="s">
-        <v>473</v>
       </c>
       <c r="F197" s="33" t="s">
         <v>62</v>
@@ -10029,9 +10029,9 @@
         <v>61</v>
       </c>
       <c r="N197" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P197" s="64">
+        <v>470</v>
+      </c>
+      <c r="P197" s="38">
         <v>801.8</v>
       </c>
       <c r="Q197">
@@ -10046,13 +10046,13 @@
         <v>336</v>
       </c>
       <c r="C198" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="D198" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="E198" t="s">
         <v>472</v>
-      </c>
-      <c r="D198" s="34" t="s">
-        <v>474</v>
-      </c>
-      <c r="E198" t="s">
-        <v>473</v>
       </c>
       <c r="F198" s="33" t="s">
         <v>62</v>
@@ -10079,9 +10079,9 @@
         <v>61</v>
       </c>
       <c r="N198" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="P198" s="64">
+        <v>470</v>
+      </c>
+      <c r="P198" s="38">
         <v>792.2</v>
       </c>
       <c r="Q198">
@@ -10712,11 +10712,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10731,6 +10726,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- fix several references in WANG2023 pointing to the paper references rather than supplement references
</commit_message>
<xml_diff>
--- a/DatasetForML_Wang2023_Hardness_CompilationAndOriginal.xlsx
+++ b/DatasetForML_Wang2023_Hardness_CompilationAndOriginal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EA7AEA-1DC3-294E-B242-28E497A06987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F4C1A-2F20-934E-BD52-0511680CA093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1358,82 +1358,7 @@
     <t>189</t>
   </si>
   <si>
-    <t>10.1016/j.mattod.2015.11.026</t>
-  </si>
-  <si>
     <t>10.1002/adem.200300567</t>
-  </si>
-  <si>
-    <t>10.1038/s41467-020-16791-8</t>
-  </si>
-  <si>
-    <t>10.1016/j.pmatsci.2022.101018</t>
-  </si>
-  <si>
-    <t>10.1007/s11837-013-0761-6</t>
-  </si>
-  <si>
-    <t>10.1039/D1EE00505G</t>
-  </si>
-  <si>
-    <t>10.1016/j.pmatsci.2013.10.001</t>
-  </si>
-  <si>
-    <t>10.1002/adem.200700240</t>
-  </si>
-  <si>
-    <t>10.1007/978-3-319-27013-5_6</t>
-  </si>
-  <si>
-    <t>10.1016/j.actamat.2016.08.081</t>
-  </si>
-  <si>
-    <t>10.1038/ncomms7529</t>
-  </si>
-  <si>
-    <t>10.1063/1.3587228</t>
-  </si>
-  <si>
-    <t>10.1177/09544062211008935</t>
-  </si>
-  <si>
-    <t>10.1007/s11837-012-0365-6</t>
-  </si>
-  <si>
-    <t>10.1016/j.matlet.2021.130368</t>
-  </si>
-  <si>
-    <t>10.1038/s41467-021-24523-9</t>
-  </si>
-  <si>
-    <t>10.1557/s43577-022-00284-8</t>
-  </si>
-  <si>
-    <t>10.1016/j.actamat.2017.08.045</t>
-  </si>
-  <si>
-    <t>10.1016/j.intermet.2016.12.007</t>
-  </si>
-  <si>
-    <t>10.1016/j.actamat.2018.07.042</t>
-  </si>
-  <si>
-    <t>10.1002/adma.202004029</t>
-  </si>
-  <si>
-    <t>10.1126/sciadv.aaz4748</t>
-  </si>
-  <si>
-    <t>10.1103/PhysRevLett.87.156401</t>
-  </si>
-  <si>
-    <t>10.1038/s41524-019-0151-x</t>
-  </si>
-  <si>
-    <t>10.1103/PhysRevLett.116.105501</t>
-  </si>
-  <si>
-    <t>10.1038/s41467-018-03846-0</t>
   </si>
   <si>
     <t>HV</t>
@@ -1584,12 +1509,87 @@
   <si>
     <t>10.1007/s11837-013-0776-z</t>
   </si>
+  <si>
+    <t>10.1016/j.msea.2010.05.052</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2016.11.376</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2019.122555</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2019.04.104</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2012.03.005</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2009.08.090</t>
+  </si>
+  <si>
+    <t>10.1016/j.jmmm.2014.07.023</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2018.07.069</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2013.01.007</t>
+  </si>
+  <si>
+    <t>10.1016/j.matlet.2006.03.140</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2012.11.074</t>
+  </si>
+  <si>
+    <t>10.1179/143307511x12998222918796</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2010.03.111</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2011.11.063</t>
+  </si>
+  <si>
+    <t>10.11890/1006-7191-122-124</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2013.09.037</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2015.07.088</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2016.06.019</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2008.07.124</t>
+  </si>
+  <si>
+    <t>10.3166/acsm.31.669-684</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2016.09.003</t>
+  </si>
+  <si>
+    <t>10.1016/j.scriptamat.2020.09.039</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2019.05.056</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2007.01.122</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2019.03.010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1673,6 +1673,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2158,7 +2164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2266,33 +2272,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2344,6 +2323,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2627,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R165" sqref="R165"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N205" sqref="N205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2664,21 +2671,21 @@
       <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="48" t="s">
-        <v>474</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="39" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2688,17 +2695,17 @@
       <c r="B3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2716,43 +2723,43 @@
       <c r="B5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="45" t="s">
-        <v>468</v>
-      </c>
-      <c r="N5" s="45" t="s">
+      <c r="M5" s="56" t="s">
+        <v>443</v>
+      </c>
+      <c r="N5" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="57" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2763,19 +2770,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="40"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2820,12 +2827,12 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="41"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="31" t="s">
-        <v>466</v>
+        <v>441</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="R7" s="23" t="s">
         <v>40</v>
@@ -2833,35 +2840,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62" t="s">
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="63"/>
+      <c r="N8" s="54"/>
       <c r="O8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="42" t="s">
+      <c r="P8" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="44"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="62"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2952,10 +2959,10 @@
         <v>42</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N10" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="P10" s="38">
         <v>220</v>
@@ -2990,10 +2997,10 @@
         <v>42</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N11" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="P11" s="38">
         <v>412</v>
@@ -3028,10 +3035,10 @@
         <v>42</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N12" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="P12" s="38">
         <v>166</v>
@@ -3066,10 +3073,10 @@
         <v>42</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N13" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="O13" s="20"/>
       <c r="P13" s="38">
@@ -3105,10 +3112,10 @@
         <v>42</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N14" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="P14" s="38">
         <v>359.6</v>
@@ -3143,10 +3150,10 @@
         <v>42</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N15" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="P15" s="38">
         <v>371.6</v>
@@ -3181,10 +3188,10 @@
         <v>42</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N16" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="P16" s="38">
         <v>386</v>
@@ -3219,10 +3226,10 @@
         <v>42</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N17" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="P17" s="38">
         <v>118</v>
@@ -3257,10 +3264,10 @@
         <v>42</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N18" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="P18" s="38">
         <v>127</v>
@@ -3295,10 +3302,10 @@
         <v>42</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N19" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="P19" s="38">
         <v>382</v>
@@ -3333,10 +3340,10 @@
         <v>42</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N20" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="P20" s="38">
         <v>527</v>
@@ -3371,10 +3378,10 @@
         <v>42</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N21" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="P21" s="38">
         <v>482</v>
@@ -3409,10 +3416,10 @@
         <v>42</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N22" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="P22" s="38">
         <v>509</v>
@@ -3447,10 +3454,10 @@
         <v>42</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N23" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="P23" s="38">
         <v>131</v>
@@ -3485,10 +3492,10 @@
         <v>42</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N24" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="P24" s="38">
         <v>388</v>
@@ -3523,10 +3530,10 @@
         <v>42</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N25" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="P25" s="38">
         <v>538</v>
@@ -3561,10 +3568,10 @@
         <v>42</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N26" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="P26" s="38">
         <v>487</v>
@@ -3599,10 +3606,10 @@
         <v>42</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N27" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="P27" s="38">
         <v>135</v>
@@ -3637,10 +3644,10 @@
         <v>42</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N28" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="P28" s="38">
         <v>205</v>
@@ -3675,10 +3682,10 @@
         <v>42</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N29" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="P29" s="38">
         <v>380</v>
@@ -3713,10 +3720,10 @@
         <v>42</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N30" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="P30" s="38">
         <v>150</v>
@@ -3751,10 +3758,10 @@
         <v>42</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N31" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="P31" s="38">
         <v>300</v>
@@ -3789,10 +3796,10 @@
         <v>42</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N32" t="s">
-        <v>445</v>
+        <v>458</v>
       </c>
       <c r="P32" s="38">
         <v>420</v>
@@ -3827,10 +3834,10 @@
         <v>42</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N33" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P33" s="38">
         <v>238</v>
@@ -3865,10 +3872,10 @@
         <v>42</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N34" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P34" s="38">
         <v>278</v>
@@ -3903,10 +3910,10 @@
         <v>42</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N35" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P35" s="38">
         <v>392</v>
@@ -3941,10 +3948,10 @@
         <v>42</v>
       </c>
       <c r="M36" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N36" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P36" s="38">
         <v>521</v>
@@ -3979,10 +3986,10 @@
         <v>42</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N37" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P37" s="38">
         <v>546</v>
@@ -4017,10 +4024,10 @@
         <v>42</v>
       </c>
       <c r="M38" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N38" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P38" s="38">
         <v>550</v>
@@ -4055,10 +4062,10 @@
         <v>42</v>
       </c>
       <c r="M39" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N39" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P39" s="38">
         <v>544</v>
@@ -4093,10 +4100,10 @@
         <v>42</v>
       </c>
       <c r="M40" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N40" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P40" s="38">
         <v>567</v>
@@ -4131,10 +4138,10 @@
         <v>42</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N41" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P41" s="38">
         <v>576</v>
@@ -4169,10 +4176,10 @@
         <v>42</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N42" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="P42" s="38">
         <v>593</v>
@@ -4207,10 +4214,10 @@
         <v>42</v>
       </c>
       <c r="M43" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N43" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P43" s="38">
         <v>473</v>
@@ -4245,10 +4252,10 @@
         <v>42</v>
       </c>
       <c r="M44" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N44" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P44" s="38">
         <v>367</v>
@@ -4283,10 +4290,10 @@
         <v>42</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N45" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P45" s="38">
         <v>458</v>
@@ -4321,10 +4328,10 @@
         <v>42</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N46" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P46" s="38">
         <v>418</v>
@@ -4359,10 +4366,10 @@
         <v>42</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N47" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P47" s="38">
         <v>423</v>
@@ -4397,10 +4404,10 @@
         <v>42</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N48" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="P48" s="38">
         <v>208</v>
@@ -4435,10 +4442,10 @@
         <v>42</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N49" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="P49" s="38">
         <v>280</v>
@@ -4473,10 +4480,10 @@
         <v>42</v>
       </c>
       <c r="M50" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N50" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="P50" s="38">
         <v>580</v>
@@ -4511,10 +4518,10 @@
         <v>42</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="N51" t="s">
-        <v>449</v>
+        <v>444</v>
+      </c>
+      <c r="N51" s="65" t="s">
+        <v>462</v>
       </c>
       <c r="P51" s="38">
         <v>450</v>
@@ -4549,10 +4556,10 @@
         <v>42</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>469</v>
-      </c>
-      <c r="N52" t="s">
-        <v>449</v>
+        <v>444</v>
+      </c>
+      <c r="N52" s="65" t="s">
+        <v>462</v>
       </c>
       <c r="P52" s="38">
         <v>304</v>
@@ -4587,10 +4594,10 @@
         <v>42</v>
       </c>
       <c r="M53" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N53" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="P53" s="38">
         <v>695</v>
@@ -4625,10 +4632,10 @@
         <v>42</v>
       </c>
       <c r="M54" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N54" t="s">
-        <v>450</v>
+        <v>463</v>
       </c>
       <c r="P54" s="38">
         <v>740</v>
@@ -4663,10 +4670,10 @@
         <v>42</v>
       </c>
       <c r="M55" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N55" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P55" s="38">
         <v>479</v>
@@ -4701,10 +4708,10 @@
         <v>42</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N56" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P56" s="38">
         <v>494</v>
@@ -4739,10 +4746,10 @@
         <v>42</v>
       </c>
       <c r="M57" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N57" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P57" s="38">
         <v>486</v>
@@ -4777,10 +4784,10 @@
         <v>42</v>
       </c>
       <c r="M58" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N58" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P58" s="38">
         <v>408</v>
@@ -4815,10 +4822,10 @@
         <v>42</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N59" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P59" s="38">
         <v>370</v>
@@ -4853,10 +4860,10 @@
         <v>42</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N60" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P60" s="38">
         <v>166</v>
@@ -4891,10 +4898,10 @@
         <v>42</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N61" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P61" s="38">
         <v>536</v>
@@ -4929,10 +4936,10 @@
         <v>42</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N62" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P62" s="38">
         <v>531</v>
@@ -4967,10 +4974,10 @@
         <v>42</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N63" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P63" s="38">
         <v>545</v>
@@ -5005,10 +5012,10 @@
         <v>42</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N64" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P64" s="38">
         <v>366</v>
@@ -5043,10 +5050,10 @@
         <v>42</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N65" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="P65" s="38">
         <v>249</v>
@@ -5081,10 +5088,10 @@
         <v>42</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N66" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P66" s="38">
         <v>178.6</v>
@@ -5119,10 +5126,10 @@
         <v>42</v>
       </c>
       <c r="M67" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N67" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P67" s="38">
         <v>169.7</v>
@@ -5157,10 +5164,10 @@
         <v>42</v>
       </c>
       <c r="M68" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N68" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P68" s="38">
         <v>182</v>
@@ -5195,10 +5202,10 @@
         <v>42</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N69" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P69" s="38">
         <v>182.5</v>
@@ -5233,10 +5240,10 @@
         <v>42</v>
       </c>
       <c r="M70" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N70" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P70" s="38">
         <v>218.9</v>
@@ -5271,10 +5278,10 @@
         <v>42</v>
       </c>
       <c r="M71" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N71" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P71" s="38">
         <v>277.8</v>
@@ -5309,10 +5316,10 @@
         <v>42</v>
       </c>
       <c r="M72" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N72" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P72" s="38">
         <v>402.6</v>
@@ -5346,10 +5353,10 @@
         <v>42</v>
       </c>
       <c r="M73" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N73" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P73" s="38">
         <v>484.1</v>
@@ -5383,10 +5390,10 @@
         <v>42</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N74" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P74" s="38">
         <v>528.29999999999995</v>
@@ -5420,10 +5427,10 @@
         <v>42</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N75" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P75" s="38">
         <v>538.1</v>
@@ -5457,10 +5464,10 @@
         <v>42</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N76" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P76" s="38">
         <v>530.29999999999995</v>
@@ -5494,10 +5501,10 @@
         <v>42</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N77" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P77" s="38">
         <v>534.20000000000005</v>
@@ -5531,10 +5538,10 @@
         <v>42</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N78" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="P78" s="38">
         <v>537.1</v>
@@ -5568,10 +5575,10 @@
         <v>42</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N79" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="P79" s="38">
         <v>168</v>
@@ -5605,10 +5612,10 @@
         <v>42</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N80" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P80" s="38">
         <v>273</v>
@@ -5642,10 +5649,10 @@
         <v>42</v>
       </c>
       <c r="M81" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N81" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P81" s="38">
         <v>475</v>
@@ -5679,10 +5686,10 @@
         <v>42</v>
       </c>
       <c r="M82" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N82" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P82" s="38">
         <v>558</v>
@@ -5716,10 +5723,10 @@
         <v>42</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N83" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P83" s="38">
         <v>510</v>
@@ -5753,10 +5760,10 @@
         <v>42</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N84" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P84" s="38">
         <v>603</v>
@@ -5790,10 +5797,10 @@
         <v>42</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N85" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P85" s="38">
         <v>625</v>
@@ -5827,10 +5834,10 @@
         <v>42</v>
       </c>
       <c r="M86" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N86" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P86" s="38">
         <v>655</v>
@@ -5864,10 +5871,10 @@
         <v>42</v>
       </c>
       <c r="M87" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N87" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="P87" s="38">
         <v>735</v>
@@ -5901,10 +5908,10 @@
         <v>42</v>
       </c>
       <c r="M88" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N88" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="P88" s="38">
         <v>152</v>
@@ -5938,10 +5945,10 @@
         <v>42</v>
       </c>
       <c r="M89" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="N89" t="s">
         <v>469</v>
-      </c>
-      <c r="N89" t="s">
-        <v>457</v>
       </c>
       <c r="P89" s="38">
         <v>286</v>
@@ -5975,10 +5982,10 @@
         <v>42</v>
       </c>
       <c r="M90" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N90" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P90" s="38">
         <v>358</v>
@@ -6012,10 +6019,10 @@
         <v>42</v>
       </c>
       <c r="M91" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N91" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P91" s="38">
         <v>586</v>
@@ -6049,10 +6056,10 @@
         <v>42</v>
       </c>
       <c r="M92" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N92" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P92" s="38">
         <v>601</v>
@@ -6086,10 +6093,10 @@
         <v>42</v>
       </c>
       <c r="M93" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N93" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P93" s="38">
         <v>295</v>
@@ -6123,10 +6130,10 @@
         <v>42</v>
       </c>
       <c r="M94" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N94" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P94" s="38">
         <v>584</v>
@@ -6160,10 +6167,10 @@
         <v>42</v>
       </c>
       <c r="M95" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N95" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P95" s="38">
         <v>310</v>
@@ -6197,10 +6204,10 @@
         <v>42</v>
       </c>
       <c r="M96" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N96" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P96" s="38">
         <v>451</v>
@@ -6234,10 +6241,10 @@
         <v>42</v>
       </c>
       <c r="M97" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N97" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P97" s="38">
         <v>546</v>
@@ -6271,10 +6278,10 @@
         <v>42</v>
       </c>
       <c r="M98" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N98" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P98" s="38">
         <v>607</v>
@@ -6308,10 +6315,10 @@
         <v>42</v>
       </c>
       <c r="M99" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N99" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P99" s="38">
         <v>537</v>
@@ -6345,10 +6352,10 @@
         <v>42</v>
       </c>
       <c r="M100" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N100" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P100" s="38">
         <v>514</v>
@@ -6382,10 +6389,10 @@
         <v>42</v>
       </c>
       <c r="M101" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N101" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P101" s="38">
         <v>604</v>
@@ -6419,10 +6426,10 @@
         <v>42</v>
       </c>
       <c r="M102" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N102" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P102" s="38">
         <v>639</v>
@@ -6456,10 +6463,10 @@
         <v>42</v>
       </c>
       <c r="M103" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N103" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P103" s="38">
         <v>534</v>
@@ -6493,10 +6500,10 @@
         <v>42</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N104" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P104" s="38">
         <v>609</v>
@@ -6530,10 +6537,10 @@
         <v>42</v>
       </c>
       <c r="M105" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N105" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P105" s="38">
         <v>551</v>
@@ -6567,10 +6574,10 @@
         <v>42</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N106" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="P106" s="38">
         <v>586</v>
@@ -6604,10 +6611,10 @@
         <v>42</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N107" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P107" s="38">
         <v>225</v>
@@ -6641,10 +6648,10 @@
         <v>42</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N108" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P108" s="38">
         <v>146</v>
@@ -6678,10 +6685,10 @@
         <v>42</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N109" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P109" s="38">
         <v>150</v>
@@ -6715,10 +6722,10 @@
         <v>42</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N110" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P110" s="38">
         <v>158</v>
@@ -6752,10 +6759,10 @@
         <v>42</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N111" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P111" s="38">
         <v>175</v>
@@ -6789,10 +6796,10 @@
         <v>42</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N112" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P112" s="38">
         <v>154</v>
@@ -6826,10 +6833,10 @@
         <v>42</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N113" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P113" s="38">
         <v>153</v>
@@ -6863,10 +6870,10 @@
         <v>42</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N114" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P114" s="38">
         <v>158</v>
@@ -6900,10 +6907,10 @@
         <v>42</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N115" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P115" s="38">
         <v>161</v>
@@ -6937,10 +6944,10 @@
         <v>42</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N116" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P116" s="38">
         <v>172</v>
@@ -6974,10 +6981,10 @@
         <v>42</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N117" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P117" s="38">
         <v>183</v>
@@ -7011,10 +7018,10 @@
         <v>42</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N118" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P118" s="38">
         <v>182</v>
@@ -7048,10 +7055,10 @@
         <v>42</v>
       </c>
       <c r="M119" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N119" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P119" s="38">
         <v>172</v>
@@ -7085,10 +7092,10 @@
         <v>42</v>
       </c>
       <c r="M120" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N120" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P120" s="38">
         <v>157</v>
@@ -7122,10 +7129,10 @@
         <v>42</v>
       </c>
       <c r="M121" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N121" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P121" s="38">
         <v>170</v>
@@ -7159,10 +7166,10 @@
         <v>42</v>
       </c>
       <c r="M122" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N122" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P122" s="38">
         <v>167</v>
@@ -7196,10 +7203,10 @@
         <v>42</v>
       </c>
       <c r="M123" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N123" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P123" s="38">
         <v>158</v>
@@ -7233,10 +7240,10 @@
         <v>42</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N124" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P124" s="38">
         <v>140</v>
@@ -7270,10 +7277,10 @@
         <v>42</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N125" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P125" s="38">
         <v>125</v>
@@ -7307,10 +7314,10 @@
         <v>42</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N126" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P126" s="38">
         <v>242</v>
@@ -7344,10 +7351,10 @@
         <v>42</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N127" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P127" s="38">
         <v>265</v>
@@ -7381,10 +7388,10 @@
         <v>42</v>
       </c>
       <c r="M128" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N128" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P128" s="38">
         <v>335</v>
@@ -7418,10 +7425,10 @@
         <v>42</v>
       </c>
       <c r="M129" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N129" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P129" s="38">
         <v>170</v>
@@ -7455,10 +7462,10 @@
         <v>42</v>
       </c>
       <c r="M130" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N130" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P130" s="38">
         <v>503</v>
@@ -7492,10 +7499,10 @@
         <v>42</v>
       </c>
       <c r="M131" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N131" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P131" s="38">
         <v>555</v>
@@ -7529,10 +7536,10 @@
         <v>42</v>
       </c>
       <c r="M132" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N132" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P132" s="38">
         <v>548</v>
@@ -7566,10 +7573,10 @@
         <v>42</v>
       </c>
       <c r="M133" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N133" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P133" s="38">
         <v>615</v>
@@ -7603,10 +7610,10 @@
         <v>42</v>
       </c>
       <c r="M134" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N134" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P134" s="38">
         <v>720</v>
@@ -7640,10 +7647,10 @@
         <v>42</v>
       </c>
       <c r="M135" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N135" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P135" s="38">
         <v>550</v>
@@ -7677,10 +7684,10 @@
         <v>42</v>
       </c>
       <c r="M136" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N136" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P136" s="38">
         <v>539</v>
@@ -7714,10 +7721,10 @@
         <v>42</v>
       </c>
       <c r="M137" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N137" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P137" s="38">
         <v>438</v>
@@ -7751,10 +7758,10 @@
         <v>42</v>
       </c>
       <c r="M138" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N138" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P138" s="38">
         <v>476</v>
@@ -7788,10 +7795,10 @@
         <v>42</v>
       </c>
       <c r="M139" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N139" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P139" s="38">
         <v>587</v>
@@ -7825,10 +7832,10 @@
         <v>42</v>
       </c>
       <c r="M140" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N140" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P140" s="38">
         <v>558</v>
@@ -7862,10 +7869,10 @@
         <v>42</v>
       </c>
       <c r="M141" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N141" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P141" s="38">
         <v>510</v>
@@ -7899,10 +7906,10 @@
         <v>42</v>
       </c>
       <c r="M142" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N142" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P142" s="38">
         <v>775</v>
@@ -7936,10 +7943,10 @@
         <v>42</v>
       </c>
       <c r="M143" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N143" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P143" s="38">
         <v>140</v>
@@ -7973,10 +7980,10 @@
         <v>42</v>
       </c>
       <c r="M144" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N144" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P144" s="38">
         <v>410</v>
@@ -8010,10 +8017,10 @@
         <v>42</v>
       </c>
       <c r="M145" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N145" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P145" s="38">
         <v>510</v>
@@ -8047,10 +8054,10 @@
         <v>42</v>
       </c>
       <c r="M146" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N146" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="P146" s="38">
         <v>145</v>
@@ -8084,10 +8091,10 @@
         <v>42</v>
       </c>
       <c r="M147" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N147" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="P147" s="38">
         <v>359</v>
@@ -8121,10 +8128,10 @@
         <v>42</v>
       </c>
       <c r="M148" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N148" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="P148" s="38">
         <v>396</v>
@@ -8158,10 +8165,10 @@
         <v>42</v>
       </c>
       <c r="M149" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N149" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P149" s="38">
         <v>271</v>
@@ -8195,10 +8202,10 @@
         <v>42</v>
       </c>
       <c r="M150" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N150" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P150" s="38">
         <v>406</v>
@@ -8232,10 +8239,10 @@
         <v>42</v>
       </c>
       <c r="M151" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N151" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P151" s="38">
         <v>481</v>
@@ -8269,10 +8276,10 @@
         <v>42</v>
       </c>
       <c r="M152" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N152" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P152" s="38">
         <v>661</v>
@@ -8306,10 +8313,10 @@
         <v>42</v>
       </c>
       <c r="M153" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N153" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P153" s="38">
         <v>240</v>
@@ -8343,10 +8350,10 @@
         <v>42</v>
       </c>
       <c r="M154" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N154" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P154" s="38">
         <v>328</v>
@@ -8380,10 +8387,10 @@
         <v>42</v>
       </c>
       <c r="M155" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N155" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P155" s="38">
         <v>379</v>
@@ -8417,10 +8424,10 @@
         <v>42</v>
       </c>
       <c r="M156" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N156" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P156" s="38">
         <v>481</v>
@@ -8454,10 +8461,10 @@
         <v>42</v>
       </c>
       <c r="M157" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N157" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P157" s="38">
         <v>484</v>
@@ -8491,10 +8498,10 @@
         <v>42</v>
       </c>
       <c r="M158" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N158" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P158" s="38">
         <v>740</v>
@@ -8528,10 +8535,10 @@
         <v>42</v>
       </c>
       <c r="M159" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N159" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P159" s="38">
         <v>169</v>
@@ -8565,10 +8572,10 @@
         <v>42</v>
       </c>
       <c r="M160" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N160" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P160" s="38">
         <v>200</v>
@@ -8602,10 +8609,10 @@
         <v>42</v>
       </c>
       <c r="M161" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N161" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P161" s="38">
         <v>240</v>
@@ -8639,10 +8646,10 @@
         <v>42</v>
       </c>
       <c r="M162" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N162" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P162" s="38">
         <v>291</v>
@@ -8676,10 +8683,10 @@
         <v>42</v>
       </c>
       <c r="M163" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N163" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P163" s="38">
         <v>322</v>
@@ -8713,10 +8720,10 @@
         <v>42</v>
       </c>
       <c r="M164" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N164" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P164" s="38">
         <v>338</v>
@@ -8750,10 +8757,10 @@
         <v>42</v>
       </c>
       <c r="M165" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N165" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P165" s="38">
         <v>389</v>
@@ -8787,10 +8794,10 @@
         <v>42</v>
       </c>
       <c r="M166" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N166" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P166" s="38">
         <v>522</v>
@@ -8824,10 +8831,10 @@
         <v>42</v>
       </c>
       <c r="M167" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N167" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P167" s="38">
         <v>572</v>
@@ -8861,10 +8868,10 @@
         <v>42</v>
       </c>
       <c r="M168" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N168" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="P168" s="38">
         <v>600</v>
@@ -8898,10 +8905,10 @@
         <v>42</v>
       </c>
       <c r="M169" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N169" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="P169" s="38">
         <v>154</v>
@@ -8935,10 +8942,10 @@
         <v>42</v>
       </c>
       <c r="M170" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N170" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="P170" s="38">
         <v>419</v>
@@ -8972,10 +8979,10 @@
         <v>42</v>
       </c>
       <c r="M171" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N171" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P171" s="38">
         <v>764</v>
@@ -9009,10 +9016,10 @@
         <v>42</v>
       </c>
       <c r="M172" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N172" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P172" s="38">
         <v>591</v>
@@ -9046,10 +9053,10 @@
         <v>42</v>
       </c>
       <c r="M173" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N173" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P173" s="38">
         <v>701</v>
@@ -9083,10 +9090,10 @@
         <v>42</v>
       </c>
       <c r="M174" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N174" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P174" s="38">
         <v>768</v>
@@ -9120,10 +9127,10 @@
         <v>42</v>
       </c>
       <c r="M175" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N175" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P175" s="38">
         <v>702</v>
@@ -9157,10 +9164,10 @@
         <v>42</v>
       </c>
       <c r="M176" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N176" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P176" s="38">
         <v>694</v>
@@ -9194,10 +9201,10 @@
         <v>42</v>
       </c>
       <c r="M177" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N177" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P177" s="38">
         <v>149</v>
@@ -9231,10 +9238,10 @@
         <v>42</v>
       </c>
       <c r="M178" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N178" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P178" s="38">
         <v>229</v>
@@ -9268,10 +9275,10 @@
         <v>42</v>
       </c>
       <c r="M179" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N179" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P179" s="38">
         <v>459</v>
@@ -9305,10 +9312,10 @@
         <v>42</v>
       </c>
       <c r="M180" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N180" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P180" s="38">
         <v>469</v>
@@ -9342,10 +9349,10 @@
         <v>42</v>
       </c>
       <c r="M181" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N181" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P181" s="38">
         <v>483</v>
@@ -9379,10 +9386,10 @@
         <v>42</v>
       </c>
       <c r="M182" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N182" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P182" s="38">
         <v>472</v>
@@ -9416,10 +9423,10 @@
         <v>42</v>
       </c>
       <c r="M183" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N183" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P183" s="38">
         <v>454</v>
@@ -9453,10 +9460,10 @@
         <v>42</v>
       </c>
       <c r="M184" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N184" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P184" s="38">
         <v>441</v>
@@ -9490,10 +9497,10 @@
         <v>42</v>
       </c>
       <c r="M185" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N185" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P185" s="38">
         <v>495</v>
@@ -9527,10 +9534,10 @@
         <v>42</v>
       </c>
       <c r="M186" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N186" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P186" s="38">
         <v>477</v>
@@ -9564,10 +9571,10 @@
         <v>42</v>
       </c>
       <c r="M187" s="20" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="N187" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="P187" s="38">
         <v>469</v>
@@ -9582,7 +9589,7 @@
       </c>
       <c r="C188" s="34"/>
       <c r="D188" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F188" s="33" t="s">
         <v>62</v>
@@ -9609,7 +9616,7 @@
         <v>61</v>
       </c>
       <c r="N188" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P188" s="38">
         <v>785.6</v>
@@ -9627,7 +9634,7 @@
       </c>
       <c r="C189" s="34"/>
       <c r="D189" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F189" s="33" t="s">
         <v>62</v>
@@ -9654,7 +9661,7 @@
         <v>61</v>
       </c>
       <c r="N189" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P189" s="38">
         <v>771.1</v>
@@ -9672,7 +9679,7 @@
       </c>
       <c r="C190" s="34"/>
       <c r="D190" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F190" s="33" t="s">
         <v>62</v>
@@ -9699,7 +9706,7 @@
         <v>61</v>
       </c>
       <c r="N190" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P190" s="38">
         <v>783.7</v>
@@ -9717,7 +9724,7 @@
       </c>
       <c r="C191" s="34"/>
       <c r="D191" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F191" s="33" t="s">
         <v>62</v>
@@ -9744,7 +9751,7 @@
         <v>61</v>
       </c>
       <c r="N191" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P191" s="38">
         <v>771.9</v>
@@ -9762,7 +9769,7 @@
       </c>
       <c r="C192" s="34"/>
       <c r="D192" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F192" s="33" t="s">
         <v>62</v>
@@ -9789,7 +9796,7 @@
         <v>61</v>
       </c>
       <c r="N192" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P192" s="38">
         <v>797.1</v>
@@ -9807,7 +9814,7 @@
       </c>
       <c r="C193" s="34"/>
       <c r="D193" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F193" s="33" t="s">
         <v>62</v>
@@ -9834,7 +9841,7 @@
         <v>61</v>
       </c>
       <c r="N193" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P193" s="38">
         <v>792.2</v>
@@ -9852,7 +9859,7 @@
       </c>
       <c r="C194" s="34"/>
       <c r="D194" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="F194" s="33" t="s">
         <v>62</v>
@@ -9879,7 +9886,7 @@
         <v>61</v>
       </c>
       <c r="N194" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P194" s="38">
         <v>804.3</v>
@@ -9896,13 +9903,13 @@
         <v>333</v>
       </c>
       <c r="C195" s="34" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="D195" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="E195" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="F195" s="33" t="s">
         <v>62</v>
@@ -9929,7 +9936,7 @@
         <v>61</v>
       </c>
       <c r="N195" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P195" s="38">
         <v>815.4</v>
@@ -9946,13 +9953,13 @@
         <v>334</v>
       </c>
       <c r="C196" s="34" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="D196" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="E196" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="F196" s="33" t="s">
         <v>62</v>
@@ -9979,7 +9986,7 @@
         <v>61</v>
       </c>
       <c r="N196" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P196" s="38">
         <v>814.5</v>
@@ -9996,13 +10003,13 @@
         <v>335</v>
       </c>
       <c r="C197" s="34" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="D197" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="E197" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="F197" s="33" t="s">
         <v>62</v>
@@ -10029,7 +10036,7 @@
         <v>61</v>
       </c>
       <c r="N197" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P197" s="38">
         <v>801.8</v>
@@ -10046,13 +10053,13 @@
         <v>336</v>
       </c>
       <c r="C198" s="34" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="D198" s="34" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="E198" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="F198" s="33" t="s">
         <v>62</v>
@@ -10079,7 +10086,7 @@
         <v>61</v>
       </c>
       <c r="N198" s="20" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="P198" s="38">
         <v>792.2</v>
@@ -10712,6 +10719,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10726,11 +10738,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>